<commit_message>
Implemented third refinement for the second exercise of nowcasting
DPG-Cap
</commit_message>
<xml_diff>
--- a/gdp_revisions_analysis_jefas/input/data/nowcasting_rel_perf.xlsx
+++ b/gdp_revisions_analysis_jefas/input/data/nowcasting_rel_perf.xlsx
@@ -83,7 +83,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>148.39120483398438</v>
+        <v>41.364051818847656</v>
       </c>
     </row>
     <row r="3">
@@ -91,7 +91,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>143.82656860351562</v>
+        <v>37.248386383056641</v>
       </c>
     </row>
     <row r="4">
@@ -99,7 +99,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>127.17751312255859</v>
+        <v>18.59356689453125</v>
       </c>
     </row>
     <row r="5">
@@ -107,7 +107,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>87.526031494140625</v>
+        <v>7.5408868789672852</v>
       </c>
     </row>
     <row r="6">
@@ -115,7 +115,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>47.085796356201172</v>
+        <v>6.0619406700134277</v>
       </c>
     </row>
     <row r="7">
@@ -123,7 +123,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>68.021408081054688</v>
+        <v>14.847681045532227</v>
       </c>
     </row>
     <row r="8">
@@ -131,7 +131,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>44.554885864257812</v>
+        <v>20.680257797241211</v>
       </c>
     </row>
     <row r="9">
@@ -139,7 +139,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>20.84794807434082</v>
+        <v>7.4842095375061035</v>
       </c>
     </row>
     <row r="10">
@@ -147,7 +147,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1">
-        <v>55.5565185546875</v>
+        <v>32.345989227294922</v>
       </c>
     </row>
     <row r="11">
@@ -155,7 +155,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1">
-        <v>97.905319213867188</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -163,7 +163,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="1">
-        <v>53.46929931640625</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>